<commit_message>
Implemented stratification into the tool
</commit_message>
<xml_diff>
--- a/jupyter_notebooks/file/input/strata_example/network.xlsx
+++ b/jupyter_notebooks/file/input/strata_example/network.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\ResiliencyTool\jupyter_notebooks\file\input\strata_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D0389F-F144-46D1-8E38-9EAC0D16D080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD807294-668E-4890-9945-013E63A0169D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
+    <workbookView xWindow="-14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="8" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
   </bookViews>
   <sheets>
     <sheet name="simulation" sheetId="12" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="166">
   <si>
     <t>name</t>
   </si>
@@ -541,10 +541,10 @@
     <t>0.2</t>
   </si>
   <si>
-    <t>dummy</t>
-  </si>
-  <si>
-    <t>tower_water</t>
+    <t>towers_1</t>
+  </si>
+  <si>
+    <t>towers_2</t>
   </si>
 </sst>
 </file>
@@ -908,15 +908,15 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>146</v>
       </c>
@@ -927,7 +927,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -942,7 +942,7 @@
         <v>44562</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>148</v>
       </c>
@@ -953,7 +953,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -964,7 +964,7 @@
         <v>44562.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>150</v>
       </c>
@@ -986,24 +986,24 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>45</v>
       </c>
@@ -1071,19 +1071,19 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>139</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>142</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>134</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>135</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>136</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>137</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>138</v>
       </c>
@@ -1333,14 +1333,14 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="9" width="12" customWidth="1"/>
-    <col min="10" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>145</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>146</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <f>DATE(2022,1,1)+TIME(0,0,0)</f>
         <v>44562</v>
@@ -1467,7 +1467,7 @@
         <v>4.27432788186315</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <f>A3+TIME(1,0,0)</f>
         <v>44562.041666666664</v>
@@ -1533,7 +1533,7 @@
         <v>5.6211919330659503</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <f t="shared" ref="A5:A50" si="9">A4+TIME(1,0,0)</f>
         <v>44562.083333333328</v>
@@ -1599,7 +1599,7 @@
         <v>1.82564940090546</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <f t="shared" si="9"/>
         <v>44562.124999999993</v>
@@ -1665,7 +1665,7 @@
         <v>3.1417148327448299</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <f t="shared" si="9"/>
         <v>44562.166666666657</v>
@@ -1731,7 +1731,7 @@
         <v>2.44040365859968</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <f t="shared" si="9"/>
         <v>44562.208333333321</v>
@@ -1797,7 +1797,7 @@
         <v>1.68806951706772</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <f t="shared" si="9"/>
         <v>44562.249999999985</v>
@@ -1863,7 +1863,7 @@
         <v>5.7615926339802899</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <f t="shared" si="9"/>
         <v>44562.29166666665</v>
@@ -1929,7 +1929,7 @@
         <v>4.4746755565582301</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <f t="shared" si="9"/>
         <v>44562.333333333314</v>
@@ -1995,7 +1995,7 @@
         <v>0.99233826848758999</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <f t="shared" si="9"/>
         <v>44562.374999999978</v>
@@ -2061,7 +2061,7 @@
         <v>1.4504413873470099</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <f t="shared" si="9"/>
         <v>44562.416666666642</v>
@@ -2127,7 +2127,7 @@
         <v>3.4424487899564999</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <f t="shared" si="9"/>
         <v>44562.458333333307</v>
@@ -2193,7 +2193,7 @@
         <v>2.8984195901566401</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <f t="shared" si="9"/>
         <v>44562.499999999971</v>
@@ -2259,7 +2259,7 @@
         <v>0.27373317868428698</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <f t="shared" si="9"/>
         <v>44562.541666666635</v>
@@ -2325,7 +2325,7 @@
         <v>2.2835876161010198</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <f t="shared" si="9"/>
         <v>44562.583333333299</v>
@@ -2391,7 +2391,7 @@
         <v>3.2042372835921999</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <f t="shared" si="9"/>
         <v>44562.624999999964</v>
@@ -2457,7 +2457,7 @@
         <v>4.3549335670475404</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <f t="shared" si="9"/>
         <v>44562.666666666628</v>
@@ -2523,7 +2523,7 @@
         <v>1.4410553784787401</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <f t="shared" si="9"/>
         <v>44562.708333333292</v>
@@ -2589,7 +2589,7 @@
         <v>1.06966709596261</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <f t="shared" si="9"/>
         <v>44562.749999999956</v>
@@ -2655,7 +2655,7 @@
         <v>2.1763329976830499</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <f t="shared" si="9"/>
         <v>44562.791666666621</v>
@@ -2721,7 +2721,7 @@
         <v>1.6300007973402</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <f t="shared" si="9"/>
         <v>44562.833333333285</v>
@@ -2787,7 +2787,7 @@
         <v>5.39135925399553</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <f t="shared" si="9"/>
         <v>44562.874999999949</v>
@@ -2853,7 +2853,7 @@
         <v>2.6246176606670999</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <f t="shared" si="9"/>
         <v>44562.916666666613</v>
@@ -2919,7 +2919,7 @@
         <v>1.7617742571331001</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <f t="shared" si="9"/>
         <v>44562.958333333278</v>
@@ -2985,7 +2985,7 @@
         <v>3.4528973487669998</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <f t="shared" si="9"/>
         <v>44562.999999999942</v>
@@ -3051,7 +3051,7 @@
         <v>4.2602474943845499</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <f t="shared" si="9"/>
         <v>44563.041666666606</v>
@@ -3117,7 +3117,7 @@
         <v>5.8161839179126202</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <f t="shared" si="9"/>
         <v>44563.08333333327</v>
@@ -3183,7 +3183,7 @@
         <v>1.46193657438067</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <f t="shared" si="9"/>
         <v>44563.124999999935</v>
@@ -3249,7 +3249,7 @@
         <v>1.6591177962361401</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <f t="shared" si="9"/>
         <v>44563.166666666599</v>
@@ -3315,7 +3315,7 @@
         <v>5.4597621212607299</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <f t="shared" si="9"/>
         <v>44563.208333333263</v>
@@ -3381,7 +3381,7 @@
         <v>1.25181920815158</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <f t="shared" si="9"/>
         <v>44563.249999999927</v>
@@ -3447,7 +3447,7 @@
         <v>3.3509127315398102</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <f t="shared" si="9"/>
         <v>44563.291666666591</v>
@@ -3513,7 +3513,7 @@
         <v>5.3115677444649299</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <f t="shared" si="9"/>
         <v>44563.333333333256</v>
@@ -3579,7 +3579,7 @@
         <v>5.4721211104801402</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <f t="shared" si="9"/>
         <v>44563.37499999992</v>
@@ -3645,7 +3645,7 @@
         <v>4.17004847290369</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <f t="shared" si="9"/>
         <v>44563.416666666584</v>
@@ -3711,7 +3711,7 @@
         <v>5.7350102271752199</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <f t="shared" si="9"/>
         <v>44563.458333333248</v>
@@ -3777,7 +3777,7 @@
         <v>3.0532018578787898</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <f t="shared" si="9"/>
         <v>44563.499999999913</v>
@@ -3843,7 +3843,7 @@
         <v>4.5127529817461802</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <f t="shared" si="9"/>
         <v>44563.541666666577</v>
@@ -3909,7 +3909,7 @@
         <v>1.81882568283527</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <f t="shared" si="9"/>
         <v>44563.583333333241</v>
@@ -3975,7 +3975,7 @@
         <v>4.1670179471692004</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <f t="shared" si="9"/>
         <v>44563.624999999905</v>
@@ -4041,7 +4041,7 @@
         <v>5.0145941909878102</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <f t="shared" si="9"/>
         <v>44563.66666666657</v>
@@ -4107,7 +4107,7 @@
         <v>4.6203567464908799</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <f t="shared" si="9"/>
         <v>44563.708333333234</v>
@@ -4173,7 +4173,7 @@
         <v>3.1860373031700502</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <f t="shared" si="9"/>
         <v>44563.749999999898</v>
@@ -4239,7 +4239,7 @@
         <v>1.4542112247108301</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <f t="shared" si="9"/>
         <v>44563.791666666562</v>
@@ -4305,7 +4305,7 @@
         <v>0.58642957599119605</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <f t="shared" si="9"/>
         <v>44563.833333333227</v>
@@ -4371,7 +4371,7 @@
         <v>2.0991375142243198</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <f t="shared" si="9"/>
         <v>44563.874999999891</v>
@@ -4437,7 +4437,7 @@
         <v>5.4879410997586398</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <f t="shared" si="9"/>
         <v>44563.916666666555</v>
@@ -4503,7 +4503,7 @@
         <v>5.0588261933592902</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <f t="shared" si="9"/>
         <v>44563.958333333219</v>
@@ -4584,27 +4584,27 @@
       <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>156</v>
       </c>
@@ -4620,12 +4620,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4636,7 +4636,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -4654,21 +4654,21 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4712,7 +4712,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -4787,7 +4787,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -4810,7 +4810,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -4833,7 +4833,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>107</v>
       </c>
@@ -4856,7 +4856,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>108</v>
       </c>
@@ -4879,7 +4879,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>109</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>110</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>111</v>
       </c>
@@ -4948,7 +4948,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>112</v>
       </c>
@@ -4971,7 +4971,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>113</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>114</v>
       </c>
@@ -5017,7 +5017,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>115</v>
       </c>
@@ -5040,7 +5040,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -5063,7 +5063,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>117</v>
       </c>
@@ -5086,7 +5086,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>132</v>
       </c>
@@ -5109,7 +5109,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>133</v>
       </c>
@@ -5141,33 +5141,33 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C68F50D-BD38-47D8-9610-A2EF7C397A58}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5216,8 +5216,11 @@
       <c r="P1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -5239,11 +5242,11 @@
       <c r="O2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="P2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -5265,11 +5268,11 @@
       <c r="O3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="P3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -5291,11 +5294,11 @@
       <c r="O4" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="P4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>134</v>
       </c>
@@ -5317,11 +5320,11 @@
       <c r="O5" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="P5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>135</v>
       </c>
@@ -5343,11 +5346,11 @@
       <c r="O6" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="P6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>136</v>
       </c>
@@ -5369,11 +5372,11 @@
       <c r="O7" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="P7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>137</v>
       </c>
@@ -5395,11 +5398,11 @@
       <c r="O8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="P8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>138</v>
       </c>
@@ -5421,8 +5424,8 @@
       <c r="O9" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="P9" t="s">
-        <v>164</v>
+      <c r="Q9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5432,41 +5435,41 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB5B7B5-BF13-4654-A134-6B30DC3D029F}">
-  <dimension ref="A1:Y8"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W1" sqref="W1"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5542,8 +5545,11 @@
       <c r="Y1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -5565,12 +5571,12 @@
       <c r="V2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="W2" t="s">
-        <v>164</v>
-      </c>
       <c r="X2" s="2"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -5592,12 +5598,12 @@
       <c r="V3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="W3" t="s">
-        <v>164</v>
-      </c>
       <c r="X3" s="2"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>139</v>
       </c>
@@ -5619,12 +5625,12 @@
       <c r="V4" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="W4" t="s">
-        <v>164</v>
-      </c>
       <c r="X4" s="2"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>140</v>
       </c>
@@ -5646,12 +5652,12 @@
       <c r="V5" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="W5" t="s">
-        <v>164</v>
-      </c>
       <c r="X5" s="2"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -5673,12 +5679,12 @@
       <c r="V6" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="W6" t="s">
-        <v>164</v>
-      </c>
       <c r="X6" s="2"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>142</v>
       </c>
@@ -5700,12 +5706,12 @@
       <c r="V7" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="W7" t="s">
-        <v>164</v>
-      </c>
       <c r="X7" s="2"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="M8" s="2"/>
       <c r="V8" s="2"/>
     </row>
@@ -5722,28 +5728,28 @@
       <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5796,7 +5802,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -5832,27 +5838,27 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5902,7 +5908,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -5959,28 +5965,28 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5FE2EA6-5FEC-471F-BC99-9A1BBFAA5478}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6014,8 +6020,11 @@
       <c r="K1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -6028,14 +6037,14 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>164</v>
-      </c>
       <c r="F2" s="2" t="s">
         <v>105</v>
       </c>
       <c r="J2">
         <v>100</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6048,31 +6057,31 @@
   <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.28515625" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.33203125" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6128,7 +6137,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -6145,9 +6154,6 @@
       <c r="E2" t="s">
         <v>45</v>
       </c>
-      <c r="K2" t="s">
-        <v>165</v>
-      </c>
       <c r="L2" s="2" t="s">
         <v>105</v>
       </c>
@@ -6170,7 +6176,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -6188,7 +6194,7 @@
         <v>45</v>
       </c>
       <c r="K3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>105</v>
@@ -6209,7 +6215,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -6248,7 +6254,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>119</v>
       </c>
@@ -6266,7 +6272,7 @@
         <v>45</v>
       </c>
       <c r="K5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>105</v>
@@ -6287,7 +6293,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>120</v>
       </c>
@@ -6305,7 +6311,7 @@
         <v>45</v>
       </c>
       <c r="K6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>105</v>
@@ -6326,7 +6332,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>121</v>
       </c>
@@ -6365,7 +6371,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>122</v>
       </c>
@@ -6404,7 +6410,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>123</v>
       </c>
@@ -6443,7 +6449,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>124</v>
       </c>
@@ -6461,7 +6467,7 @@
         <v>45</v>
       </c>
       <c r="K10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>105</v>
@@ -6483,7 +6489,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>125</v>
       </c>
@@ -6500,9 +6506,6 @@
       <c r="E11" t="s">
         <v>45</v>
       </c>
-      <c r="K11" t="s">
-        <v>165</v>
-      </c>
       <c r="L11" s="2" t="s">
         <v>105</v>
       </c>
@@ -6522,7 +6525,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>126</v>
       </c>
@@ -6540,7 +6543,7 @@
         <v>45</v>
       </c>
       <c r="K12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>105</v>
@@ -6561,7 +6564,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>127</v>
       </c>
@@ -6579,7 +6582,7 @@
         <v>45</v>
       </c>
       <c r="K13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>105</v>
@@ -6600,7 +6603,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>128</v>
       </c>
@@ -6639,7 +6642,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>129</v>
       </c>
@@ -6678,7 +6681,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>130</v>
       </c>
@@ -6695,9 +6698,6 @@
       <c r="E16" t="s">
         <v>45</v>
       </c>
-      <c r="K16" t="s">
-        <v>165</v>
-      </c>
       <c r="L16" s="2" t="s">
         <v>105</v>
       </c>
@@ -6717,7 +6717,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>131</v>
       </c>
@@ -6733,9 +6733,6 @@
       </c>
       <c r="E17" t="s">
         <v>45</v>
-      </c>
-      <c r="K17" t="s">
-        <v>165</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
Added the possibility for multiple return periods
</commit_message>
<xml_diff>
--- a/jupyter_notebooks/file/input/strata_example/network.xlsx
+++ b/jupyter_notebooks/file/input/strata_example/network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\ResiliencyTool\jupyter_notebooks\file\input\strata_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD807294-668E-4890-9945-013E63A0169D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CDD9CB-1EF6-47E1-9938-7A689701BF5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="8" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="8" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
   </bookViews>
   <sheets>
     <sheet name="simulation" sheetId="12" r:id="rId1"/>
@@ -22,10 +22,11 @@
     <sheet name="tr_type" sheetId="6" r:id="rId7"/>
     <sheet name="transformers" sheetId="3" r:id="rId8"/>
     <sheet name="lines" sheetId="4" r:id="rId9"/>
-    <sheet name="ln_type" sheetId="7" r:id="rId10"/>
-    <sheet name="cost" sheetId="10" r:id="rId11"/>
-    <sheet name="profiles" sheetId="11" r:id="rId12"/>
-    <sheet name="crews" sheetId="13" r:id="rId13"/>
+    <sheet name="switches" sheetId="14" r:id="rId10"/>
+    <sheet name="ln_type" sheetId="7" r:id="rId11"/>
+    <sheet name="cost" sheetId="10" r:id="rId12"/>
+    <sheet name="profiles" sheetId="11" r:id="rId13"/>
+    <sheet name="crews" sheetId="13" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="179">
   <si>
     <t>name</t>
   </si>
@@ -545,6 +546,45 @@
   </si>
   <si>
     <t>towers_2</t>
+  </si>
+  <si>
+    <t>element</t>
+  </si>
+  <si>
+    <t>et</t>
+  </si>
+  <si>
+    <t>in_ka</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>associated elements</t>
+  </si>
+  <si>
+    <t>ignore montecarlo</t>
+  </si>
+  <si>
+    <t>return_period</t>
+  </si>
+  <si>
+    <t>rp1</t>
+  </si>
+  <si>
+    <t>rp2</t>
+  </si>
+  <si>
+    <t>rp3</t>
+  </si>
+  <si>
+    <t>rp4</t>
+  </si>
+  <si>
+    <t>rp5</t>
+  </si>
+  <si>
+    <t>rp6</t>
   </si>
 </sst>
 </file>
@@ -982,6 +1022,103 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F048EE5-6CF5-4D91-BE31-E59CF33F6687}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B643028-F04F-4526-8B5B-4E99E7FCEC09}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1063,7 +1200,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03625BB4-D62C-4FF6-AAD9-1E9790CBA541}">
   <dimension ref="A1:H16"/>
   <sheetViews>
@@ -1325,7 +1462,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF69C053-E8BE-41F5-B9A4-E34E9036274A}">
   <dimension ref="A1:U50"/>
   <sheetViews>
@@ -4576,7 +4713,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA625533-3B9A-44F8-8593-9BC4C933B1AA}">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -5435,10 +5572,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB5B7B5-BF13-4654-A134-6B30DC3D029F}">
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5469,7 +5606,7 @@
     <col min="25" max="25" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5548,8 +5685,11 @@
       <c r="Z1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -5576,7 +5716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -5603,7 +5743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>139</v>
       </c>
@@ -5630,7 +5770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>140</v>
       </c>
@@ -5657,7 +5797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -5684,7 +5824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>142</v>
       </c>
@@ -5711,7 +5851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="M8" s="2"/>
       <c r="V8" s="2"/>
     </row>
@@ -5965,10 +6105,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5FE2EA6-5FEC-471F-BC99-9A1BBFAA5478}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5986,7 +6126,7 @@
     <col min="11" max="11" width="2.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6023,8 +6163,11 @@
       <c r="L1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -6054,10 +6197,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA2B7A3-5BF0-4668-9FF0-C3329253032F}">
-  <dimension ref="A1:U17"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6079,9 +6222,10 @@
     <col min="15" max="15" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6136,8 +6280,11 @@
       <c r="R1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -6148,7 +6295,6 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <f>U2*$T$2</f>
         <v>35</v>
       </c>
       <c r="E2" t="s">
@@ -6169,14 +6315,8 @@
       <c r="R2" t="s">
         <v>163</v>
       </c>
-      <c r="T2">
-        <v>0.5</v>
-      </c>
-      <c r="U2">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -6187,7 +6327,6 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D17" si="0">U3*$T$2</f>
         <v>25</v>
       </c>
       <c r="E3" t="s">
@@ -6211,11 +6350,11 @@
       <c r="R3" t="s">
         <v>163</v>
       </c>
-      <c r="U3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -6226,7 +6365,6 @@
         <v>106</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
         <v>20.5</v>
       </c>
       <c r="E4" t="s">
@@ -6250,11 +6388,11 @@
       <c r="R4" t="s">
         <v>163</v>
       </c>
-      <c r="U4">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>119</v>
       </c>
@@ -6265,7 +6403,6 @@
         <v>107</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="E5" t="s">
@@ -6289,11 +6426,11 @@
       <c r="R5" t="s">
         <v>163</v>
       </c>
-      <c r="U5">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>120</v>
       </c>
@@ -6304,7 +6441,6 @@
         <v>108</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
         <v>21.5</v>
       </c>
       <c r="E6" t="s">
@@ -6328,11 +6464,11 @@
       <c r="R6" t="s">
         <v>163</v>
       </c>
-      <c r="U6">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>121</v>
       </c>
@@ -6343,7 +6479,6 @@
         <v>109</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="E7" t="s">
@@ -6367,11 +6502,11 @@
       <c r="R7" t="s">
         <v>163</v>
       </c>
-      <c r="U7">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>122</v>
       </c>
@@ -6382,7 +6517,6 @@
         <v>110</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
         <v>22.5</v>
       </c>
       <c r="E8" t="s">
@@ -6406,11 +6540,11 @@
       <c r="R8" t="s">
         <v>163</v>
       </c>
-      <c r="U8">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>123</v>
       </c>
@@ -6421,7 +6555,6 @@
         <v>133</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="E9" t="s">
@@ -6445,11 +6578,11 @@
       <c r="R9" t="s">
         <v>163</v>
       </c>
-      <c r="U9">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>124</v>
       </c>
@@ -6460,7 +6593,6 @@
         <v>111</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
         <v>23.5</v>
       </c>
       <c r="E10" t="s">
@@ -6485,11 +6617,11 @@
       <c r="R10" t="s">
         <v>163</v>
       </c>
-      <c r="U10">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>125</v>
       </c>
@@ -6500,7 +6632,6 @@
         <v>112</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="E11" t="s">
@@ -6521,11 +6652,8 @@
       <c r="R11" t="s">
         <v>163</v>
       </c>
-      <c r="U11">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>126</v>
       </c>
@@ -6536,7 +6664,6 @@
         <v>113</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
         <v>24.5</v>
       </c>
       <c r="E12" t="s">
@@ -6560,11 +6687,11 @@
       <c r="R12" t="s">
         <v>163</v>
       </c>
-      <c r="U12">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>127</v>
       </c>
@@ -6575,7 +6702,6 @@
         <v>114</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="E13" t="s">
@@ -6599,11 +6725,11 @@
       <c r="R13" t="s">
         <v>163</v>
       </c>
-      <c r="U13">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>128</v>
       </c>
@@ -6614,7 +6740,6 @@
         <v>115</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
         <v>25.5</v>
       </c>
       <c r="E14" t="s">
@@ -6638,11 +6763,11 @@
       <c r="R14" t="s">
         <v>163</v>
       </c>
-      <c r="U14">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>129</v>
       </c>
@@ -6653,7 +6778,6 @@
         <v>116</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="E15" t="s">
@@ -6677,11 +6801,11 @@
       <c r="R15" t="s">
         <v>163</v>
       </c>
-      <c r="U15">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>130</v>
       </c>
@@ -6692,7 +6816,6 @@
         <v>117</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
         <v>26.5</v>
       </c>
       <c r="E16" t="s">
@@ -6713,11 +6836,8 @@
       <c r="R16" t="s">
         <v>163</v>
       </c>
-      <c r="U16">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>131</v>
       </c>
@@ -6728,7 +6848,6 @@
         <v>132</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="E17" t="s">
@@ -6748,9 +6867,6 @@
       </c>
       <c r="R17" t="s">
         <v>163</v>
-      </c>
-      <c r="U17">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added stratas to the output table and updated KPI calculation
</commit_message>
<xml_diff>
--- a/jupyter_notebooks/file/input/strata_example/network.xlsx
+++ b/jupyter_notebooks/file/input/strata_example/network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\ResiliencyTool\jupyter_notebooks\file\input\strata_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CDD9CB-1EF6-47E1-9938-7A689701BF5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0EAD03-9378-4FD3-B0C8-1A67292BB04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="8" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
   </bookViews>
   <sheets>
     <sheet name="simulation" sheetId="12" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="181">
   <si>
     <t>name</t>
   </si>
@@ -585,6 +585,12 @@
   </si>
   <si>
     <t>rp6</t>
+  </si>
+  <si>
+    <t>gen_1</t>
+  </si>
+  <si>
+    <t>gen_2</t>
   </si>
 </sst>
 </file>
@@ -948,15 +954,15 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>146</v>
       </c>
@@ -967,7 +973,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -982,7 +988,7 @@
         <v>44562</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>148</v>
       </c>
@@ -993,7 +999,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -1004,7 +1010,7 @@
         <v>44562.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>150</v>
       </c>
@@ -1029,15 +1035,15 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1066,50 +1072,50 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
@@ -1126,21 +1132,21 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1175,7 +1181,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>45</v>
       </c>
@@ -1208,19 +1214,19 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1246,7 +1252,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1260,7 +1266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1274,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1288,7 +1294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>139</v>
       </c>
@@ -1302,7 +1308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -1316,7 +1322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -1330,7 +1336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>142</v>
       </c>
@@ -1344,7 +1350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1358,7 +1364,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1372,7 +1378,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1386,7 +1392,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>134</v>
       </c>
@@ -1400,7 +1406,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>135</v>
       </c>
@@ -1414,7 +1420,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>136</v>
       </c>
@@ -1428,7 +1434,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>137</v>
       </c>
@@ -1442,7 +1448,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>138</v>
       </c>
@@ -1470,14 +1476,14 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="9" width="12" customWidth="1"/>
-    <col min="10" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>145</v>
       </c>
@@ -1506,7 +1512,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>146</v>
       </c>
@@ -1535,7 +1541,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f>DATE(2022,1,1)+TIME(0,0,0)</f>
         <v>44562</v>
@@ -1604,7 +1610,7 @@
         <v>4.27432788186315</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <f>A3+TIME(1,0,0)</f>
         <v>44562.041666666664</v>
@@ -1670,7 +1676,7 @@
         <v>5.6211919330659503</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f t="shared" ref="A5:A50" si="9">A4+TIME(1,0,0)</f>
         <v>44562.083333333328</v>
@@ -1736,7 +1742,7 @@
         <v>1.82564940090546</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <f t="shared" si="9"/>
         <v>44562.124999999993</v>
@@ -1802,7 +1808,7 @@
         <v>3.1417148327448299</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f t="shared" si="9"/>
         <v>44562.166666666657</v>
@@ -1868,7 +1874,7 @@
         <v>2.44040365859968</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" si="9"/>
         <v>44562.208333333321</v>
@@ -1934,7 +1940,7 @@
         <v>1.68806951706772</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f t="shared" si="9"/>
         <v>44562.249999999985</v>
@@ -2000,7 +2006,7 @@
         <v>5.7615926339802899</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f t="shared" si="9"/>
         <v>44562.29166666665</v>
@@ -2066,7 +2072,7 @@
         <v>4.4746755565582301</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <f t="shared" si="9"/>
         <v>44562.333333333314</v>
@@ -2132,7 +2138,7 @@
         <v>0.99233826848758999</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <f t="shared" si="9"/>
         <v>44562.374999999978</v>
@@ -2198,7 +2204,7 @@
         <v>1.4504413873470099</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <f t="shared" si="9"/>
         <v>44562.416666666642</v>
@@ -2264,7 +2270,7 @@
         <v>3.4424487899564999</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <f t="shared" si="9"/>
         <v>44562.458333333307</v>
@@ -2330,7 +2336,7 @@
         <v>2.8984195901566401</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <f t="shared" si="9"/>
         <v>44562.499999999971</v>
@@ -2396,7 +2402,7 @@
         <v>0.27373317868428698</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <f t="shared" si="9"/>
         <v>44562.541666666635</v>
@@ -2462,7 +2468,7 @@
         <v>2.2835876161010198</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <f t="shared" si="9"/>
         <v>44562.583333333299</v>
@@ -2528,7 +2534,7 @@
         <v>3.2042372835921999</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <f t="shared" si="9"/>
         <v>44562.624999999964</v>
@@ -2594,7 +2600,7 @@
         <v>4.3549335670475404</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <f t="shared" si="9"/>
         <v>44562.666666666628</v>
@@ -2660,7 +2666,7 @@
         <v>1.4410553784787401</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <f t="shared" si="9"/>
         <v>44562.708333333292</v>
@@ -2726,7 +2732,7 @@
         <v>1.06966709596261</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <f t="shared" si="9"/>
         <v>44562.749999999956</v>
@@ -2792,7 +2798,7 @@
         <v>2.1763329976830499</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <f t="shared" si="9"/>
         <v>44562.791666666621</v>
@@ -2858,7 +2864,7 @@
         <v>1.6300007973402</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <f t="shared" si="9"/>
         <v>44562.833333333285</v>
@@ -2924,7 +2930,7 @@
         <v>5.39135925399553</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <f t="shared" si="9"/>
         <v>44562.874999999949</v>
@@ -2990,7 +2996,7 @@
         <v>2.6246176606670999</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <f t="shared" si="9"/>
         <v>44562.916666666613</v>
@@ -3056,7 +3062,7 @@
         <v>1.7617742571331001</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <f t="shared" si="9"/>
         <v>44562.958333333278</v>
@@ -3122,7 +3128,7 @@
         <v>3.4528973487669998</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <f t="shared" si="9"/>
         <v>44562.999999999942</v>
@@ -3188,7 +3194,7 @@
         <v>4.2602474943845499</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <f t="shared" si="9"/>
         <v>44563.041666666606</v>
@@ -3254,7 +3260,7 @@
         <v>5.8161839179126202</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <f t="shared" si="9"/>
         <v>44563.08333333327</v>
@@ -3320,7 +3326,7 @@
         <v>1.46193657438067</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <f t="shared" si="9"/>
         <v>44563.124999999935</v>
@@ -3386,7 +3392,7 @@
         <v>1.6591177962361401</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <f t="shared" si="9"/>
         <v>44563.166666666599</v>
@@ -3452,7 +3458,7 @@
         <v>5.4597621212607299</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <f t="shared" si="9"/>
         <v>44563.208333333263</v>
@@ -3518,7 +3524,7 @@
         <v>1.25181920815158</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <f t="shared" si="9"/>
         <v>44563.249999999927</v>
@@ -3584,7 +3590,7 @@
         <v>3.3509127315398102</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <f t="shared" si="9"/>
         <v>44563.291666666591</v>
@@ -3650,7 +3656,7 @@
         <v>5.3115677444649299</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <f t="shared" si="9"/>
         <v>44563.333333333256</v>
@@ -3716,7 +3722,7 @@
         <v>5.4721211104801402</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <f t="shared" si="9"/>
         <v>44563.37499999992</v>
@@ -3782,7 +3788,7 @@
         <v>4.17004847290369</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <f t="shared" si="9"/>
         <v>44563.416666666584</v>
@@ -3848,7 +3854,7 @@
         <v>5.7350102271752199</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <f t="shared" si="9"/>
         <v>44563.458333333248</v>
@@ -3914,7 +3920,7 @@
         <v>3.0532018578787898</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <f t="shared" si="9"/>
         <v>44563.499999999913</v>
@@ -3980,7 +3986,7 @@
         <v>4.5127529817461802</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <f t="shared" si="9"/>
         <v>44563.541666666577</v>
@@ -4046,7 +4052,7 @@
         <v>1.81882568283527</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <f t="shared" si="9"/>
         <v>44563.583333333241</v>
@@ -4112,7 +4118,7 @@
         <v>4.1670179471692004</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <f t="shared" si="9"/>
         <v>44563.624999999905</v>
@@ -4178,7 +4184,7 @@
         <v>5.0145941909878102</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <f t="shared" si="9"/>
         <v>44563.66666666657</v>
@@ -4244,7 +4250,7 @@
         <v>4.6203567464908799</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <f t="shared" si="9"/>
         <v>44563.708333333234</v>
@@ -4310,7 +4316,7 @@
         <v>3.1860373031700502</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <f t="shared" si="9"/>
         <v>44563.749999999898</v>
@@ -4376,7 +4382,7 @@
         <v>1.4542112247108301</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <f t="shared" si="9"/>
         <v>44563.791666666562</v>
@@ -4442,7 +4448,7 @@
         <v>0.58642957599119605</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <f t="shared" si="9"/>
         <v>44563.833333333227</v>
@@ -4508,7 +4514,7 @@
         <v>2.0991375142243198</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <f t="shared" si="9"/>
         <v>44563.874999999891</v>
@@ -4574,7 +4580,7 @@
         <v>5.4879410997586398</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <f t="shared" si="9"/>
         <v>44563.916666666555</v>
@@ -4640,7 +4646,7 @@
         <v>5.0588261933592902</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <f t="shared" si="9"/>
         <v>44563.958333333219</v>
@@ -4721,27 +4727,27 @@
       <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>156</v>
       </c>
@@ -4760,9 +4766,9 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4773,7 +4779,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -4794,18 +4800,18 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" customWidth="1"/>
-    <col min="11" max="11" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4849,7 +4855,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4878,7 +4884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -4901,7 +4907,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -4924,7 +4930,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -4947,7 +4953,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -4970,7 +4976,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>107</v>
       </c>
@@ -4993,7 +4999,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>108</v>
       </c>
@@ -5016,7 +5022,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>109</v>
       </c>
@@ -5039,7 +5045,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>110</v>
       </c>
@@ -5062,7 +5068,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>111</v>
       </c>
@@ -5085,7 +5091,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>112</v>
       </c>
@@ -5108,7 +5114,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>113</v>
       </c>
@@ -5131,7 +5137,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>114</v>
       </c>
@@ -5154,7 +5160,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>115</v>
       </c>
@@ -5177,7 +5183,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -5200,7 +5206,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>117</v>
       </c>
@@ -5223,7 +5229,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>132</v>
       </c>
@@ -5246,7 +5252,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>133</v>
       </c>
@@ -5284,27 +5290,27 @@
       <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5357,7 +5363,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -5383,7 +5389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -5409,7 +5415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -5435,7 +5441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>134</v>
       </c>
@@ -5461,7 +5467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>135</v>
       </c>
@@ -5487,7 +5493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>136</v>
       </c>
@@ -5513,7 +5519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>137</v>
       </c>
@@ -5539,7 +5545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>138</v>
       </c>
@@ -5574,39 +5580,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB5B7B5-BF13-4654-A134-6B30DC3D029F}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5689,7 +5696,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -5710,13 +5717,19 @@
       </c>
       <c r="V2" s="2" t="s">
         <v>105</v>
+      </c>
+      <c r="W2" t="s">
+        <v>179</v>
       </c>
       <c r="X2" s="2"/>
       <c r="Z2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -5737,13 +5750,19 @@
       </c>
       <c r="V3" s="2" t="s">
         <v>105</v>
+      </c>
+      <c r="W3" t="s">
+        <v>180</v>
       </c>
       <c r="X3" s="2"/>
       <c r="Z3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>139</v>
       </c>
@@ -5770,7 +5789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>140</v>
       </c>
@@ -5791,13 +5810,19 @@
       </c>
       <c r="V5" s="2" t="s">
         <v>105</v>
+      </c>
+      <c r="W5" t="s">
+        <v>179</v>
       </c>
       <c r="X5" s="2"/>
       <c r="Z5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -5818,13 +5843,19 @@
       </c>
       <c r="V6" s="2" t="s">
         <v>105</v>
+      </c>
+      <c r="W6" t="s">
+        <v>180</v>
       </c>
       <c r="X6" s="2"/>
       <c r="Z6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>142</v>
       </c>
@@ -5851,7 +5882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="M8" s="2"/>
       <c r="V8" s="2"/>
     </row>
@@ -5868,28 +5899,28 @@
       <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5942,7 +5973,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -5978,27 +6009,27 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6048,7 +6079,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -6111,22 +6142,22 @@
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6167,7 +6198,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -6199,33 +6230,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA2B7A3-5BF0-4668-9FF0-C3329253032F}">
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.33203125" customWidth="1"/>
-    <col min="14" max="14" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.28515625" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6284,7 +6315,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -6316,7 +6347,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -6354,7 +6385,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -6392,7 +6423,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>119</v>
       </c>
@@ -6430,7 +6461,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>120</v>
       </c>
@@ -6468,7 +6499,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>121</v>
       </c>
@@ -6506,7 +6537,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>122</v>
       </c>
@@ -6544,7 +6575,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>123</v>
       </c>
@@ -6582,7 +6613,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>124</v>
       </c>
@@ -6621,7 +6652,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>125</v>
       </c>
@@ -6653,7 +6684,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>126</v>
       </c>
@@ -6691,7 +6722,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>127</v>
       </c>
@@ -6729,7 +6760,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>128</v>
       </c>
@@ -6767,7 +6798,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>129</v>
       </c>
@@ -6805,7 +6836,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>130</v>
       </c>
@@ -6837,7 +6868,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>131</v>
       </c>

</xml_diff>

<commit_message>
Update docs, looking for error in module
</commit_message>
<xml_diff>
--- a/jupyter_notebooks/file/input/strata_example/network.xlsx
+++ b/jupyter_notebooks/file/input/strata_example/network.xlsx
@@ -1,32 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mn6461\Documents\GitHub\reXplan-repo\jupyter_notebooks\file\input\strata_example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engie-my.sharepoint.com/personal/mn6461_engie_com/Documents/Dokumente/GitHub/reXplan-repo/jupyter_notebooks/file/input/strata_example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FDA946-708A-40FE-A73D-3A4343A8A34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="152" documentId="13_ncr:1_{46FDA946-708A-40FE-A73D-3A4343A8A34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3F64CF4-8018-478B-892F-CFCAF861A5E1}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-8940" windowWidth="25440" windowHeight="15390" firstSheet="1" activeTab="2" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
+    <workbookView xWindow="-25320" yWindow="-8805" windowWidth="25440" windowHeight="15270" firstSheet="5" activeTab="12" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
   </bookViews>
   <sheets>
     <sheet name="simulation" sheetId="12" r:id="rId1"/>
     <sheet name="network" sheetId="5" r:id="rId2"/>
     <sheet name="nodes" sheetId="1" r:id="rId3"/>
-    <sheet name="loads" sheetId="8" r:id="rId4"/>
-    <sheet name="generators" sheetId="2" r:id="rId5"/>
-    <sheet name="external_gen" sheetId="9" r:id="rId6"/>
-    <sheet name="tr_type" sheetId="6" r:id="rId7"/>
-    <sheet name="transformers" sheetId="3" r:id="rId8"/>
-    <sheet name="lines" sheetId="4" r:id="rId9"/>
-    <sheet name="switches" sheetId="14" r:id="rId10"/>
-    <sheet name="ln_type" sheetId="7" r:id="rId11"/>
-    <sheet name="cost" sheetId="10" r:id="rId12"/>
-    <sheet name="profiles" sheetId="11" r:id="rId13"/>
-    <sheet name="crews" sheetId="13" r:id="rId14"/>
+    <sheet name="static_generators" sheetId="15" r:id="rId4"/>
+    <sheet name="loads" sheetId="8" r:id="rId5"/>
+    <sheet name="generators" sheetId="2" r:id="rId6"/>
+    <sheet name="external_gen" sheetId="9" r:id="rId7"/>
+    <sheet name="tr_type" sheetId="6" r:id="rId8"/>
+    <sheet name="transformers" sheetId="3" r:id="rId9"/>
+    <sheet name="lines" sheetId="4" r:id="rId10"/>
+    <sheet name="switches" sheetId="14" r:id="rId11"/>
+    <sheet name="ln_type" sheetId="7" r:id="rId12"/>
+    <sheet name="cost" sheetId="10" r:id="rId13"/>
+    <sheet name="profiles" sheetId="11" r:id="rId14"/>
+    <sheet name="crews" sheetId="13" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="182">
   <si>
     <t>name</t>
   </si>
@@ -591,6 +592,9 @@
   </si>
   <si>
     <t>gen_2</t>
+  </si>
+  <si>
+    <t>False</t>
   </si>
 </sst>
 </file>
@@ -683,6 +687,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1028,6 +1036,687 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA2B7A3-5BF0-4668-9FF0-C3329253032F}">
+  <dimension ref="A1:S17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.33203125" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R1" t="s">
+        <v>162</v>
+      </c>
+      <c r="S1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2">
+        <v>100</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" t="s">
+        <v>164</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O3">
+        <v>100</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>4</v>
+      </c>
+      <c r="R3" t="s">
+        <v>163</v>
+      </c>
+      <c r="S3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4">
+        <v>20.5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" t="s">
+        <v>165</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O4">
+        <v>100</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>3</v>
+      </c>
+      <c r="R4" t="s">
+        <v>163</v>
+      </c>
+      <c r="S4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" t="s">
+        <v>164</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O5">
+        <v>100</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>3</v>
+      </c>
+      <c r="R5" t="s">
+        <v>163</v>
+      </c>
+      <c r="S5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6">
+        <v>21.5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" t="s">
+        <v>164</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O6">
+        <v>100</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>3</v>
+      </c>
+      <c r="R6" t="s">
+        <v>163</v>
+      </c>
+      <c r="S6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" t="s">
+        <v>165</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O7">
+        <v>100</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7" t="s">
+        <v>163</v>
+      </c>
+      <c r="S7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8">
+        <v>22.5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" t="s">
+        <v>165</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O8">
+        <v>100</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>2</v>
+      </c>
+      <c r="R8" t="s">
+        <v>163</v>
+      </c>
+      <c r="S8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" t="s">
+        <v>165</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O9">
+        <v>100</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9" t="s">
+        <v>163</v>
+      </c>
+      <c r="S9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10">
+        <v>23.5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" t="s">
+        <v>164</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N10" s="7"/>
+      <c r="O10">
+        <v>100</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10" t="s">
+        <v>163</v>
+      </c>
+      <c r="S10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O11">
+        <v>100</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12">
+        <v>24.5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="K12" t="s">
+        <v>164</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O12">
+        <v>100</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>3</v>
+      </c>
+      <c r="R12" t="s">
+        <v>163</v>
+      </c>
+      <c r="S12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K13" t="s">
+        <v>164</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O13">
+        <v>100</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>3</v>
+      </c>
+      <c r="R13" t="s">
+        <v>163</v>
+      </c>
+      <c r="S13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14">
+        <v>25.5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="K14" t="s">
+        <v>165</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O14">
+        <v>100</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>4</v>
+      </c>
+      <c r="R14" t="s">
+        <v>163</v>
+      </c>
+      <c r="S14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15">
+        <v>26</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="K15" t="s">
+        <v>165</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O15">
+        <v>100</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15" t="s">
+        <v>163</v>
+      </c>
+      <c r="S15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16">
+        <v>26.5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O16">
+        <v>100</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17">
+        <v>27</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O17">
+        <v>100</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>2</v>
+      </c>
+      <c r="R17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F048EE5-6CF5-4D91-BE31-E59CF33F6687}">
   <dimension ref="A1:I11"/>
   <sheetViews>
@@ -1124,7 +1813,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B643028-F04F-4526-8B5B-4E99E7FCEC09}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1206,12 +1895,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03625BB4-D62C-4FF6-AAD9-1E9790CBA541}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1262,9 +1951,6 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1276,9 +1962,6 @@
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1290,9 +1973,6 @@
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1304,9 +1984,6 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1318,9 +1995,6 @@
       <c r="C6">
         <v>0</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1332,9 +2006,6 @@
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -1346,9 +2017,6 @@
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1360,9 +2028,6 @@
       <c r="C9">
         <v>-1</v>
       </c>
-      <c r="E9">
-        <v>-1</v>
-      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1374,9 +2039,6 @@
       <c r="C10">
         <v>-1</v>
       </c>
-      <c r="E10">
-        <v>-1</v>
-      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -1388,9 +2050,6 @@
       <c r="C11">
         <v>-1</v>
       </c>
-      <c r="E11">
-        <v>-1</v>
-      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1402,9 +2061,6 @@
       <c r="C12">
         <v>-1</v>
       </c>
-      <c r="E12">
-        <v>-1</v>
-      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1416,9 +2072,6 @@
       <c r="C13">
         <v>-1</v>
       </c>
-      <c r="E13">
-        <v>-1</v>
-      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1430,9 +2083,6 @@
       <c r="C14">
         <v>-1</v>
       </c>
-      <c r="E14">
-        <v>-1</v>
-      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1444,9 +2094,6 @@
       <c r="C15">
         <v>-1</v>
       </c>
-      <c r="E15">
-        <v>-1</v>
-      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1456,9 +2103,6 @@
         <v>160</v>
       </c>
       <c r="C16">
-        <v>-1</v>
-      </c>
-      <c r="E16">
         <v>-1</v>
       </c>
     </row>
@@ -1468,7 +2112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF69C053-E8BE-41F5-B9A4-E34E9036274A}">
   <dimension ref="A1:U50"/>
   <sheetViews>
@@ -4719,7 +5363,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA625533-3B9A-44F8-8593-9BC4C933B1AA}">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -4796,7 +5440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:E19"/>
     </sheetView>
   </sheetViews>
@@ -5283,6 +5927,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CAB804-19BD-4952-91D3-41A2BA646418}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C68F50D-BD38-47D8-9610-A2EF7C397A58}">
   <dimension ref="A1:Q9"/>
   <sheetViews>
@@ -5576,12 +6234,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB5B7B5-BF13-4654-A134-6B30DC3D029F}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AB6" sqref="AB6"/>
+    <sheetView topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="V7" sqref="V2:V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5716,7 +6374,7 @@
         <v>105</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>105</v>
+        <v>181</v>
       </c>
       <c r="W2" t="s">
         <v>179</v>
@@ -5749,7 +6407,7 @@
         <v>105</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>105</v>
+        <v>181</v>
       </c>
       <c r="W3" t="s">
         <v>180</v>
@@ -5782,7 +6440,7 @@
         <v>105</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>105</v>
+        <v>181</v>
       </c>
       <c r="X4" s="2"/>
       <c r="Z4">
@@ -5809,7 +6467,7 @@
         <v>105</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>105</v>
+        <v>181</v>
       </c>
       <c r="W5" t="s">
         <v>179</v>
@@ -5842,7 +6500,7 @@
         <v>105</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>105</v>
+        <v>181</v>
       </c>
       <c r="W6" t="s">
         <v>180</v>
@@ -5875,7 +6533,7 @@
         <v>105</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>105</v>
+        <v>181</v>
       </c>
       <c r="X7" s="2"/>
       <c r="Z7">
@@ -5891,7 +6549,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06392EB3-C4FB-4DF3-BD7E-3D0934814FDF}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -6001,7 +6659,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD17E09-C6E9-4EE3-B588-F4BAB32A1513}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -6134,7 +6792,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5FE2EA6-5FEC-471F-BC99-9A1BBFAA5478}">
   <dimension ref="A1:M2"/>
   <sheetViews>
@@ -6226,687 +6884,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA2B7A3-5BF0-4668-9FF0-C3329253032F}">
-  <dimension ref="A1:S17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.33203125" customWidth="1"/>
-    <col min="14" max="14" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P1" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>158</v>
-      </c>
-      <c r="R1" t="s">
-        <v>162</v>
-      </c>
-      <c r="S1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O2">
-        <v>100</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" t="s">
-        <v>164</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O3">
-        <v>100</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>4</v>
-      </c>
-      <c r="R3" t="s">
-        <v>163</v>
-      </c>
-      <c r="S3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4">
-        <v>20.5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" t="s">
-        <v>165</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O4">
-        <v>100</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>3</v>
-      </c>
-      <c r="R4" t="s">
-        <v>163</v>
-      </c>
-      <c r="S4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" t="s">
-        <v>164</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O5">
-        <v>100</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>3</v>
-      </c>
-      <c r="R5" t="s">
-        <v>163</v>
-      </c>
-      <c r="S5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6">
-        <v>21.5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" t="s">
-        <v>164</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O6">
-        <v>100</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>3</v>
-      </c>
-      <c r="R6" t="s">
-        <v>163</v>
-      </c>
-      <c r="S6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>121</v>
-      </c>
-      <c r="B7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>45</v>
-      </c>
-      <c r="K7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O7">
-        <v>100</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="R7" t="s">
-        <v>163</v>
-      </c>
-      <c r="S7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8">
-        <v>22.5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8" t="s">
-        <v>165</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O8">
-        <v>100</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>2</v>
-      </c>
-      <c r="R8" t="s">
-        <v>163</v>
-      </c>
-      <c r="S8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B9" t="s">
-        <v>109</v>
-      </c>
-      <c r="C9" t="s">
-        <v>133</v>
-      </c>
-      <c r="D9">
-        <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K9" t="s">
-        <v>165</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O9">
-        <v>100</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-      <c r="R9" t="s">
-        <v>163</v>
-      </c>
-      <c r="S9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10">
-        <v>23.5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K10" t="s">
-        <v>164</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="N10" s="7"/>
-      <c r="O10">
-        <v>100</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>1</v>
-      </c>
-      <c r="R10" t="s">
-        <v>163</v>
-      </c>
-      <c r="S10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D11">
-        <v>24</v>
-      </c>
-      <c r="E11" t="s">
-        <v>45</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O11">
-        <v>100</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>126</v>
-      </c>
-      <c r="B12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12">
-        <v>24.5</v>
-      </c>
-      <c r="E12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K12" t="s">
-        <v>164</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O12">
-        <v>100</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>3</v>
-      </c>
-      <c r="R12" t="s">
-        <v>163</v>
-      </c>
-      <c r="S12" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>127</v>
-      </c>
-      <c r="B13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C13" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13">
-        <v>25</v>
-      </c>
-      <c r="E13" t="s">
-        <v>45</v>
-      </c>
-      <c r="K13" t="s">
-        <v>164</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O13">
-        <v>100</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>3</v>
-      </c>
-      <c r="R13" t="s">
-        <v>163</v>
-      </c>
-      <c r="S13" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>128</v>
-      </c>
-      <c r="B14" t="s">
-        <v>114</v>
-      </c>
-      <c r="C14" t="s">
-        <v>115</v>
-      </c>
-      <c r="D14">
-        <v>25.5</v>
-      </c>
-      <c r="E14" t="s">
-        <v>45</v>
-      </c>
-      <c r="K14" t="s">
-        <v>165</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O14">
-        <v>100</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <v>4</v>
-      </c>
-      <c r="R14" t="s">
-        <v>163</v>
-      </c>
-      <c r="S14" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>129</v>
-      </c>
-      <c r="B15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C15" t="s">
-        <v>116</v>
-      </c>
-      <c r="D15">
-        <v>26</v>
-      </c>
-      <c r="E15" t="s">
-        <v>45</v>
-      </c>
-      <c r="K15" t="s">
-        <v>165</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O15">
-        <v>100</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>1</v>
-      </c>
-      <c r="R15" t="s">
-        <v>163</v>
-      </c>
-      <c r="S15" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>130</v>
-      </c>
-      <c r="B16" t="s">
-        <v>116</v>
-      </c>
-      <c r="C16" t="s">
-        <v>117</v>
-      </c>
-      <c r="D16">
-        <v>26.5</v>
-      </c>
-      <c r="E16" t="s">
-        <v>45</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O16">
-        <v>100</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>131</v>
-      </c>
-      <c r="B17" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" t="s">
-        <v>132</v>
-      </c>
-      <c r="D17">
-        <v>27</v>
-      </c>
-      <c r="E17" t="s">
-        <v>45</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O17">
-        <v>100</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>2</v>
-      </c>
-      <c r="R17" t="s">
-        <v>163</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{c135c4ba-2280-41f8-be7d-6f21d368baa3}" enabled="1" method="Standard" siteId="{24139d14-c62c-4c47-8bdd-ce71ea1d50cf}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
Add fragility curve data and improve interpolation method handling
</commit_message>
<xml_diff>
--- a/jupyter_notebooks/file/input/strata_example/network.xlsx
+++ b/jupyter_notebooks/file/input/strata_example/network.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\ResiliencyTool\jupyter_notebooks\file\input\strata_example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\reXplan-repo\jupyter_notebooks\file\input\strata_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0EAD03-9378-4FD3-B0C8-1A67292BB04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485C4974-CFFA-4C11-8DD9-292384562AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
   </bookViews>
   <sheets>
     <sheet name="simulation" sheetId="12" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="183">
   <si>
     <t>name</t>
   </si>
@@ -591,6 +591,12 @@
   </si>
   <si>
     <t>gen_2</t>
+  </si>
+  <si>
+    <t>interpolation method</t>
+  </si>
+  <si>
+    <t>0: Step - 1: Linear - 2: Polynomial</t>
   </si>
 </sst>
 </file>
@@ -948,15 +954,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7CE9D1-E831-4D14-93C0-93FEACE3FE30}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
@@ -1019,6 +1025,20 @@
       </c>
       <c r="C5">
         <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -5580,8 +5600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB5B7B5-BF13-4654-A134-6B30DC3D029F}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AB6" sqref="AB6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Re-worked the creation of pandapower network (pp_network). All pandapower parameters are now imported to rexplan
</commit_message>
<xml_diff>
--- a/jupyter_notebooks/file/input/strata_example/network.xlsx
+++ b/jupyter_notebooks/file/input/strata_example/network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\reXplan-repo\jupyter_notebooks\file\input\strata_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485C4974-CFFA-4C11-8DD9-292384562AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31E0E80-A2AD-4894-8900-E71B98DE7609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
+    <workbookView xWindow="6825" yWindow="5010" windowWidth="28365" windowHeight="15345" firstSheet="8" activeTab="8" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
   </bookViews>
   <sheets>
     <sheet name="simulation" sheetId="12" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="182">
   <si>
     <t>name</t>
   </si>
@@ -515,12 +515,6 @@
     <t>crew_1</t>
   </si>
   <si>
-    <t>crew_2</t>
-  </si>
-  <si>
-    <t>crew_3</t>
-  </si>
-  <si>
     <t>failureProb</t>
   </si>
   <si>
@@ -597,6 +591,9 @@
   </si>
   <si>
     <t>0: Step - 1: Linear - 2: Polynomial</t>
+  </si>
+  <si>
+    <t>priority</t>
   </si>
 </sst>
 </file>
@@ -956,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7CE9D1-E831-4D14-93C0-93FEACE3FE30}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +996,7 @@
         <v>148</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C3">
         <v>40</v>
@@ -1021,7 +1018,7 @@
         <v>150</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -1029,16 +1026,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1071,25 +1068,25 @@
         <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
       </c>
       <c r="F1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" t="s">
         <v>168</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>169</v>
-      </c>
-      <c r="H1" t="s">
-        <v>170</v>
-      </c>
-      <c r="I1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1375,7 +1372,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C9">
         <v>-1</v>
@@ -1389,7 +1386,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C10">
         <v>-1</v>
@@ -1403,7 +1400,7 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C11">
         <v>-1</v>
@@ -1417,7 +1414,7 @@
         <v>134</v>
       </c>
       <c r="B12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C12">
         <v>-1</v>
@@ -1431,7 +1428,7 @@
         <v>135</v>
       </c>
       <c r="B13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -1445,7 +1442,7 @@
         <v>136</v>
       </c>
       <c r="B14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C14">
         <v>-1</v>
@@ -1459,7 +1456,7 @@
         <v>137</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -1473,7 +1470,7 @@
         <v>138</v>
       </c>
       <c r="B16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C16">
         <v>-1</v>
@@ -4741,10 +4738,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA625533-3B9A-44F8-8593-9BC4C933B1AA}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4760,16 +4757,6 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -5380,7 +5367,7 @@
         <v>101</v>
       </c>
       <c r="Q1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -5698,7 +5685,7 @@
         <v>92</v>
       </c>
       <c r="V1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="W1" t="s">
         <v>101</v>
@@ -5710,10 +5697,10 @@
         <v>86</v>
       </c>
       <c r="Z1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AA1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
@@ -5739,14 +5726,14 @@
         <v>105</v>
       </c>
       <c r="W2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="X2" s="2"/>
       <c r="Z2">
         <v>1</v>
       </c>
       <c r="AA2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -5772,14 +5759,14 @@
         <v>105</v>
       </c>
       <c r="W3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="X3" s="2"/>
       <c r="Z3">
         <v>1</v>
       </c>
       <c r="AA3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
@@ -5832,14 +5819,14 @@
         <v>105</v>
       </c>
       <c r="W5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="X5" s="2"/>
       <c r="Z5">
         <v>1</v>
       </c>
       <c r="AA5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
@@ -5865,14 +5852,14 @@
         <v>105</v>
       </c>
       <c r="W6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="X6" s="2"/>
       <c r="Z6">
         <v>1</v>
       </c>
       <c r="AA6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
@@ -6212,10 +6199,10 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -6248,10 +6235,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA2B7A3-5BF0-4668-9FF0-C3329253032F}">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6274,9 +6261,10 @@
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6323,19 +6311,22 @@
         <v>35</v>
       </c>
       <c r="P1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="Q1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="R1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="S1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="T1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -6364,10 +6355,13 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="T2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -6384,7 +6378,7 @@
         <v>45</v>
       </c>
       <c r="K3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>105</v>
@@ -6399,13 +6393,16 @@
         <v>4</v>
       </c>
       <c r="R3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="T3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -6422,7 +6419,7 @@
         <v>45</v>
       </c>
       <c r="K4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>105</v>
@@ -6437,13 +6434,16 @@
         <v>3</v>
       </c>
       <c r="R4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="T4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>119</v>
       </c>
@@ -6460,7 +6460,7 @@
         <v>45</v>
       </c>
       <c r="K5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>105</v>
@@ -6475,13 +6475,16 @@
         <v>3</v>
       </c>
       <c r="R5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="T5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>120</v>
       </c>
@@ -6498,7 +6501,7 @@
         <v>45</v>
       </c>
       <c r="K6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>105</v>
@@ -6513,13 +6516,16 @@
         <v>3</v>
       </c>
       <c r="R6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="T6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>121</v>
       </c>
@@ -6536,7 +6542,7 @@
         <v>45</v>
       </c>
       <c r="K7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>105</v>
@@ -6551,13 +6557,16 @@
         <v>1</v>
       </c>
       <c r="R7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="T7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>122</v>
       </c>
@@ -6574,7 +6583,7 @@
         <v>45</v>
       </c>
       <c r="K8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>105</v>
@@ -6589,13 +6598,16 @@
         <v>2</v>
       </c>
       <c r="R8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="T8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>123</v>
       </c>
@@ -6612,7 +6624,7 @@
         <v>45</v>
       </c>
       <c r="K9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>105</v>
@@ -6627,13 +6639,16 @@
         <v>1</v>
       </c>
       <c r="R9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="T9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>124</v>
       </c>
@@ -6650,7 +6665,7 @@
         <v>45</v>
       </c>
       <c r="K10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>105</v>
@@ -6666,13 +6681,16 @@
         <v>1</v>
       </c>
       <c r="R10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="T10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>125</v>
       </c>
@@ -6701,10 +6719,13 @@
         <v>0</v>
       </c>
       <c r="R11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="T11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>126</v>
       </c>
@@ -6721,7 +6742,7 @@
         <v>45</v>
       </c>
       <c r="K12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>105</v>
@@ -6736,13 +6757,16 @@
         <v>3</v>
       </c>
       <c r="R12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S12" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="T12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>127</v>
       </c>
@@ -6759,7 +6783,7 @@
         <v>45</v>
       </c>
       <c r="K13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>105</v>
@@ -6774,13 +6798,16 @@
         <v>3</v>
       </c>
       <c r="R13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S13" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="T13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>128</v>
       </c>
@@ -6797,7 +6824,7 @@
         <v>45</v>
       </c>
       <c r="K14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>105</v>
@@ -6812,13 +6839,16 @@
         <v>4</v>
       </c>
       <c r="R14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S14" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="T14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>129</v>
       </c>
@@ -6835,7 +6865,7 @@
         <v>45</v>
       </c>
       <c r="K15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>105</v>
@@ -6850,13 +6880,16 @@
         <v>1</v>
       </c>
       <c r="R15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S15" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+      <c r="T15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>130</v>
       </c>
@@ -6885,10 +6918,13 @@
         <v>0</v>
       </c>
       <c r="R16" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="T16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>131</v>
       </c>
@@ -6917,7 +6953,10 @@
         <v>2</v>
       </c>
       <c r="R17" t="s">
-        <v>163</v>
+        <v>161</v>
+      </c>
+      <c r="T17">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>